<commit_message>
ED targets file added
</commit_message>
<xml_diff>
--- a/chemtest_complex.xlsx
+++ b/chemtest_complex.xlsx
@@ -20,51 +20,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t xml:space="preserve">chembl_id</t>
   </si>
   <si>
-    <t xml:space="preserve">dummy1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dummy2</t>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">species</t>
   </si>
   <si>
     <t xml:space="preserve">CHEMBL230</t>
   </si>
   <si>
-    <t xml:space="preserve">dc11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dc12</t>
+    <t xml:space="preserve">Cyclooxygenase-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homo sapiens</t>
   </si>
   <si>
     <t xml:space="preserve">CHEMBL25</t>
   </si>
   <si>
-    <t xml:space="preserve">dc21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dc22</t>
+    <t xml:space="preserve">aspirin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">na</t>
   </si>
   <si>
     <t xml:space="preserve">CHEMBL4523582</t>
   </si>
   <si>
-    <t xml:space="preserve">dc31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dc32</t>
+    <t xml:space="preserve">Replicase polyprotein 1ab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Severe acute respiratory syndrome coronavirus 2 </t>
   </si>
   <si>
     <t xml:space="preserve">CHEMBL3616356</t>
   </si>
   <si>
-    <t xml:space="preserve">dc41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dc42</t>
+    <t xml:space="preserve">D-aspartate oxidase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rattus norvegicus </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHEMBL1871</t>
+  </si>
+  <si>
+    <t xml:space="preserve">androgen receptor</t>
   </si>
 </sst>
 </file>
@@ -139,9 +145,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -165,16 +175,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.3"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.74"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -188,11 +199,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="0" t="s">
@@ -200,36 +211,47 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>